<commit_message>
updated and completed code
</commit_message>
<xml_diff>
--- a/Ictinternship/src/test/resources/TestExcel.xlsx
+++ b/Ictinternship/src/test/resources/TestExcel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projectworkspace\Ictinternship\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\githubrepo\Ictinternship\Ictinternship\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA609D6-BA37-42AA-834F-D08BE4783694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DC02C6-ADF5-4DC8-A189-ADC9CC12438F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,30 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>princy@gmail.com</t>
   </si>
   <si>
-    <t>arjun@gmail.com</t>
-  </si>
-  <si>
-    <t>salman@gmail.com</t>
-  </si>
-  <si>
-    <t>fathima@gmail.com</t>
-  </si>
-  <si>
     <t>project1</t>
-  </si>
-  <si>
-    <t>project2</t>
-  </si>
-  <si>
-    <t>project3</t>
-  </si>
-  <si>
-    <t>project4</t>
   </si>
 </sst>
 </file>
@@ -377,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,48 +378,18 @@
         <v>123456</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>123456</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>123456</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>123456</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{6C478D4F-3642-4239-A9DB-DB801CCA84A3}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{625C132A-1C51-451A-B087-617ED0659EBA}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{C797D862-C89F-4343-B8AB-92DCD0FA6C4F}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{074F0352-4588-4E51-9175-1A55CFCD8A3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>